<commit_message>
updated sens analysis tool for final trade-off
</commit_message>
<xml_diff>
--- a/tradeoff/tradeOffInput.xlsx
+++ b/tradeoff/tradeOffInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Coding/Python/Workspaces/DSE-07/tradeoff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AB22AD-C8D6-9F4B-8F30-CC4C8B1FD6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CCA43D-F31E-1241-8475-C5FF1913BB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23600" yWindow="3740" windowWidth="23600" windowHeight="15900" activeTab="2" xr2:uid="{B8562684-D365-4D40-81D0-666B8A340FBD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{B8562684-D365-4D40-81D0-666B8A340FBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Concepts" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Concept ID</t>
   </si>
@@ -68,24 +68,6 @@
     <t>Concept Name</t>
   </si>
   <si>
-    <t>Ballistic Hydrolox Jarvis</t>
-  </si>
-  <si>
-    <t>Ballistic Methalox Jarvis</t>
-  </si>
-  <si>
-    <t>Gliding Hydrolox Starship</t>
-  </si>
-  <si>
-    <t>Gliding Methalox Starship</t>
-  </si>
-  <si>
-    <t>Gliding Hydrolox Spaceplane</t>
-  </si>
-  <si>
-    <t>Gliding Methalox Spaceplane</t>
-  </si>
-  <si>
     <t>Criteria</t>
   </si>
   <si>
@@ -102,6 +84,18 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Polar Bear</t>
+  </si>
+  <si>
+    <t>Grizzly Bear</t>
+  </si>
+  <si>
+    <t>Beluga</t>
+  </si>
+  <si>
+    <t>Dolphin</t>
   </si>
 </sst>
 </file>
@@ -473,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE83EC7C-0936-E343-9148-3F38B90D2169}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,7 +488,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -502,7 +496,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -510,7 +504,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -518,23 +512,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -547,49 +525,49 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -599,10 +577,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52FF4CC-201E-BC4A-8046-25FA9D7C0CC2}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,28 +600,28 @@
         <v>Emissions</v>
       </c>
       <c r="D1" t="str">
+        <v>Cost</v>
+      </c>
+      <c r="E1" t="str">
         <v>Risk</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Cost</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" cm="1">
-        <f t="array" ref="A2:A7">Concepts!A2:A7</f>
+        <f t="array" ref="A2:A5">Concepts!A2:A5</f>
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -651,16 +629,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -668,16 +646,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
       <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
         <v>1</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -688,47 +666,13 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final version of sens analysis used for midterm
</commit_message>
<xml_diff>
--- a/tradeoff/tradeOffInput.xlsx
+++ b/tradeoff/tradeOffInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Coding/Python/Workspaces/DSE-07/tradeoff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CCA43D-F31E-1241-8475-C5FF1913BB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9012EBCF-12DA-354F-9AB1-48922B2D7ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{B8562684-D365-4D40-81D0-666B8A340FBD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -102,13 +102,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,8 +137,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,7 +532,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,7 +566,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -567,7 +574,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -580,7 +587,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,33 +618,33 @@
         <f t="array" ref="A2:A5">Concepts!A2:A5</f>
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="1">
         <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>5</v>
       </c>
     </row>
@@ -645,16 +652,16 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>1</v>
       </c>
     </row>
@@ -662,17 +669,17 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>3</v>
       </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>